<commit_message>
Ajout des services en ligne
</commit_message>
<xml_diff>
--- a/Documents Excel/etatDesLieuxIntranetDuCHIC.xlsx
+++ b/Documents Excel/etatDesLieuxIntranetDuCHIC.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
-  <si>
-    <t>A la découverte du CHIC</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="94">
   <si>
     <t>Le livret d'accueil du personnel</t>
   </si>
@@ -38,9 +35,6 @@
     <t>A Valider</t>
   </si>
   <si>
-    <t>Responsable</t>
-  </si>
-  <si>
     <t>Commentaires</t>
   </si>
   <si>
@@ -117,9 +111,6 @@
   </si>
   <si>
     <t>pdf (15 Décembre 2020)</t>
-  </si>
-  <si>
-    <t>Commetaires</t>
   </si>
   <si>
     <t>Documentation Externe Générale</t>
@@ -248,9 +239,6 @@
 propose</t>
   </si>
   <si>
-    <t>Qui est Responsable ?</t>
-  </si>
-  <si>
     <t>10 PDFs : 1. Journal Officiel de la République Française (3 mai 2005)</t>
   </si>
   <si>
@@ -270,6 +258,57 @@
   </si>
   <si>
     <t>DOCUMENTATION</t>
+  </si>
+  <si>
+    <t>SERVICES EN LIGNE</t>
+  </si>
+  <si>
+    <t>ScanRisk</t>
+  </si>
+  <si>
+    <t>Agenda partagé</t>
+  </si>
+  <si>
+    <t>SILLAGE RDV Web</t>
+  </si>
+  <si>
+    <t>SILLAGE RDV Lien sur l’accès agenda mode Web</t>
+  </si>
+  <si>
+    <t>Responsable ?</t>
+  </si>
+  <si>
+    <t>SILLAGE CENTRE HOSPITALIER de DOUARNENEZ Michel Mazeas</t>
+  </si>
+  <si>
+    <t>Tableau de bord opérationnels des services du CHIC</t>
+  </si>
+  <si>
+    <t>THESAURUS des diagnostiques et des actes</t>
+  </si>
+  <si>
+    <t>THYMUS</t>
+  </si>
+  <si>
+    <t>Les Conventions du CHIC</t>
+  </si>
+  <si>
+    <t>PENELOPE - SACSO - GASP</t>
+  </si>
+  <si>
+    <t>Commande des repas pour les patients - laisser ses coordonnées</t>
+  </si>
+  <si>
+    <t>Site inaccessible</t>
+  </si>
+  <si>
+    <t>Lien ne fonctionne pas sur Chrome</t>
+  </si>
+  <si>
+    <t>Fichier ou répertoire introuvable (404)</t>
+  </si>
+  <si>
+    <t>Exception Oracle</t>
   </si>
 </sst>
 </file>
@@ -394,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -430,14 +469,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -720,54 +756,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="40.140625" customWidth="1"/>
-    <col min="6" max="6" width="65.85546875" customWidth="1"/>
+    <col min="1" max="1" width="60.5703125" customWidth="1"/>
+    <col min="2" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="58.42578125" customWidth="1"/>
+    <col min="6" max="6" width="74.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -777,35 +818,35 @@
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -815,115 +856,115 @@
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="16"/>
       <c r="F8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="16"/>
       <c r="F10" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="16"/>
       <c r="F11" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="16"/>
       <c r="F12" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="16"/>
       <c r="F13" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="16"/>
       <c r="F14" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="16"/>
       <c r="F15" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="16"/>
       <c r="F16" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -933,7 +974,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -943,51 +984,41 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="16"/>
       <c r="F20" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>6</v>
-      </c>
+      <c r="A21" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>32</v>
+      <c r="A22" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -997,100 +1028,100 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1102,8 +1133,8 @@
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="20" t="s">
-        <v>46</v>
+      <c r="A32" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1113,179 +1144,325 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
       <c r="F40" s="14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="18" t="s">
-        <v>66</v>
+      <c r="F43" s="17" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="16"/>
       <c r="F44" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="16"/>
       <c r="F45" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="16"/>
-      <c r="F46" s="19" t="s">
-        <v>72</v>
-      </c>
+      <c r="F46" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>81</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F52" s="1"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F53" s="1"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>86</v>
+      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>87</v>
+      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>89</v>
+      </c>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Ajout des services fonctionnels
</commit_message>
<xml_diff>
--- a/Documents Excel/etatDesLieuxIntranetDuCHIC.xlsx
+++ b/Documents Excel/etatDesLieuxIntranetDuCHIC.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="130">
   <si>
     <t>Le livret d'accueil du personnel</t>
   </si>
@@ -260,9 +260,6 @@
     <t>DOCUMENTATION</t>
   </si>
   <si>
-    <t>SERVICES EN LIGNE</t>
-  </si>
-  <si>
     <t>ScanRisk</t>
   </si>
   <si>
@@ -309,13 +306,124 @@
   </si>
   <si>
     <t>Exception Oracle</t>
+  </si>
+  <si>
+    <t>SERVICES EN LIGNE (qui ne fonctionnent pas actuellement)</t>
+  </si>
+  <si>
+    <t>SERVICES EN LIGNE (fonctionnels)</t>
+  </si>
+  <si>
+    <t>Manuel unique du laboratoire</t>
+  </si>
+  <si>
+    <t>COPILOTE PUI Web - Commande de médicaments</t>
+  </si>
+  <si>
+    <t>COPILOTE PUI Web - Module de traçabilité</t>
+  </si>
+  <si>
+    <t>COPILOTE DRM</t>
+  </si>
+  <si>
+    <t>Chimio Web</t>
+  </si>
+  <si>
+    <t>Référentiel des anti-infectieux</t>
+  </si>
+  <si>
+    <t>Accès Logiciel du Temps de Travail (CHRONOS)</t>
+  </si>
+  <si>
+    <t>Accès Logiciel du Temps de Travail Médical (eGTT)</t>
+  </si>
+  <si>
+    <t>Accès Gestion Documentaire du Patient</t>
+  </si>
+  <si>
+    <t>Accès logiciel PTAH : Demandes de transports pédestres</t>
+  </si>
+  <si>
+    <t>Accès au logiciel ALFA LIMA : Saisie des demandes d'admission en SSR</t>
+  </si>
+  <si>
+    <t>Accès au logiciel OPTIM Commandes</t>
+  </si>
+  <si>
+    <t>GESFORM : Formation Continue</t>
+  </si>
+  <si>
+    <t>DRM : Dépôt de commandes</t>
+  </si>
+  <si>
+    <t>Matelas à Air : Accès à la commande en ligne</t>
+  </si>
+  <si>
+    <t>VIDOC : Gardes Cadres de Santé</t>
+  </si>
+  <si>
+    <t>VACTUS : Espace Collaboratif</t>
+  </si>
+  <si>
+    <t>VDG : Dépôt documents gériatres du pôle personnes âgées</t>
+  </si>
+  <si>
+    <t>RESA : Occupation - Réservation des Salles utilisables</t>
+  </si>
+  <si>
+    <t>STUdS</t>
+  </si>
+  <si>
+    <t>Accès au CLASSEUR (rangement documents)</t>
+  </si>
+  <si>
+    <t>Accès à l'agenda partagé</t>
+  </si>
+  <si>
+    <t>RUBIS</t>
+  </si>
+  <si>
+    <t>Pilotage Medico-économique</t>
+  </si>
+  <si>
+    <t>CertDc</t>
+  </si>
+  <si>
+    <t>GENOIS</t>
+  </si>
+  <si>
+    <t>VIDAL</t>
+  </si>
+  <si>
+    <t>Soumettre une demande de sossiers médicaux par mail</t>
+  </si>
+  <si>
+    <t>Chirurgie Réservation des Lits</t>
+  </si>
+  <si>
+    <t>Hôpital de Jour Médecine</t>
+  </si>
+  <si>
+    <t>Hôpital de Semaine Médecine</t>
+  </si>
+  <si>
+    <t>Hôpital de Semaine Cardiologie</t>
+  </si>
+  <si>
+    <t>Hôpital de Jour Rééducation Quimper</t>
+  </si>
+  <si>
+    <t>Hôpital de Jour Addictologie le Porzou</t>
+  </si>
+  <si>
+    <t>Hôpital de Jour de Pediatrie</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,6 +467,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -433,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -476,6 +590,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -756,15 +871,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.5703125" customWidth="1"/>
+    <col min="1" max="1" width="62.28515625" customWidth="1"/>
     <col min="2" max="3" width="12.5703125" customWidth="1"/>
     <col min="4" max="4" width="22.140625" customWidth="1"/>
     <col min="5" max="5" width="58.42578125" customWidth="1"/>
@@ -787,7 +902,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>3</v>
@@ -830,7 +945,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -854,7 +969,7 @@
       <c r="E7" s="16"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -902,7 +1017,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>16</v>
       </c>
@@ -914,7 +1029,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
@@ -1310,7 +1425,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1320,19 +1435,19 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1342,114 +1457,116 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F50" s="1"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F53" s="1"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F55" s="1"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F56" s="1"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F58" s="1"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
+      <c r="A59" s="10" t="s">
+        <v>94</v>
+      </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -1457,12 +1574,362 @@
       <c r="F59" s="1"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
+      <c r="A60" s="20" t="s">
+        <v>95</v>
+      </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>